<commit_message>
updated data generation with the isVersionOf attribute
</commit_message>
<xml_diff>
--- a/C_LDES/vkb_example.xlsx
+++ b/C_LDES/vkb_example.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,11 @@
           <t>doelAssetId.identificator</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>http://purl.org/dc/terms/isVersionOf</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -526,6 +531,11 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>aanzicht_01</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>https://data.awvvlaanderen.be/id/asset/HeeftAanzicht_-_opstelling_01_-_aanzicht_01</t>
         </is>
       </c>
     </row>
@@ -535,109 +545,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="20" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>typeURI</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assetId.identificator</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assetId.toegekendDoor</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>assetVersie.context</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>assetVersie.timestamp</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>assetVersie.versienummer</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/implementatieelement#RelatieObject.bron</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/implementatieelement#RelatieObject.doel</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#HoortBij</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>HoortBij_-_bord_01_-_aanzicht_01</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>OTLMOW</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>DA_Init</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2021-01-01 00:00:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://data.awvvlaanderen.be/id/asset/bord_01</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>https://data.awvvlaanderen.be/id/asset/aanzicht_01</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -684,23 +591,141 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>hoek</t>
+          <t>http://purl.org/dc/terms/isVersionOf</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>isActief</t>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/implementatieelement#RelatieObject.bron</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>toestand</t>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/implementatieelement#RelatieObject.doel</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#HoortBij</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>HoortBij_-_bord_01_-_aanzicht_01</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OTLMOW</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>DA_Init</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2021-01-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://data.awvvlaanderen.be/id/asset/HoortBij_-_bord_01_-_aanzicht_01</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://data.awvvlaanderen.be/id/asset/bord_01</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://data.awvvlaanderen.be/id/asset/aanzicht_01</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="20" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>typeURI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assetId.identificator</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assetId.toegekendDoor</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>assetVersie.context</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>assetVersie.timestamp</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>assetVersie.versienummer</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>hoek</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>http://purl.org/dc/terms/isVersionOf</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>isActief</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>toestand</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>https://wegenenverkeer.data.vlaanderen.be/ns/installatie#AanzichtVerkeersbordopstelling</t>
         </is>
       </c>
@@ -732,10 +757,15 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>https://data.awvvlaanderen.be/id/asset/aanzicht_01</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>True</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>in-gebruik</t>
         </is>
@@ -752,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,15 +828,20 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>http://purl.org/dc/terms/isVersionOf</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>isActief</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>opstelhoogte</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>toestand</t>
         </is>
@@ -846,11 +881,16 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>https://data.awvvlaanderen.be/id/asset/bord_01</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>True</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
         <is>
           <t>in-ontwerp</t>
         </is>
@@ -890,15 +930,20 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>https://data.awvvlaanderen.be/id/asset/bord_01</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>True</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>1.8</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>in-gebruik</t>
         </is>
@@ -915,7 +960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,10 +1006,15 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>http://purl.org/dc/terms/isVersionOf</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>isActief</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>toestand</t>
         </is>
@@ -1004,10 +1054,15 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>https://data.awvvlaanderen.be/id/asset/opstelling_01</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>True</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>in-gebruik</t>
         </is>

</xml_diff>